<commit_message>
update 31 linh kiện, tbi
</commit_message>
<xml_diff>
--- a/VatTuRobotTuDong2026.xlsx
+++ b/VatTuRobotTuDong2026.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a34dd17289f0cd43/文档/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\DanhSachVatTu_Robocon2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{88072F2D-98B1-4917-AE78-CA8B73A92C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74BFEB6C-4982-44A7-A8EA-B9E121F95544}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB37D47D-9D1A-4315-BE6E-458899B68014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B568294B-4D84-4998-9F35-E8011388998F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
   <si>
     <t>STT</t>
   </si>
@@ -743,6 +743,33 @@
   </si>
   <si>
     <t>Dự trù vật tư điện cho Robot Tự Động Robocon 2026</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>https://www.anphatpc.com.vn/o-cung-western-digital-black-sn7100-1tb-m2-pcie-nvme-gen-4-4-wds100t4x0e.html</t>
+  </si>
+  <si>
+    <t>https://www.anphatpc.com.vn/ram-laptop-kingston-16gb-ddr4-bus-3200-kvr32s22d8/16wp.html</t>
+  </si>
+  <si>
+    <t>Kích thước: M.2 2280
+Giao diện: PCIe Gen4.0 x4/5.0 x2, NVMe 2.0
+Dung lượng: 1TB
+Tốc độ đọc/ghi (up to ): 7,150 MB/s - 6,300 MB/s
+Tốc độ đọc/ghi 4K (4KB, QD32) up to: 850,000 IOPS - 1,350,000 IOP
+Kiểu Flash: Samsung V-NAND TLC</t>
+  </si>
+  <si>
+    <t>Dung lượng: 16GB
+Bus: 3200Mhz
+Độ trễ: CL22
+Điện áp: 1.2V
+Tản nhiệt: Không</t>
   </si>
 </sst>
 </file>
@@ -968,9 +995,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,6 +1016,9 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -999,322 +1026,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0\ &quot;₫&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1421,6 +1132,303 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0\ &quot;₫&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1446,6 +1454,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1822,13 +1849,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>278778</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2689858</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>2518407</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1944,13 +1971,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>52024</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>10841</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2949529</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>2010364</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2066,13 +2093,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>49191</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2914648</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2346959</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2127,13 +2154,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>210949</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2916555</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>2306955</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2188,13 +2215,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2838696</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>2646045</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2249,13 +2276,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>53541</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2948940</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>2914650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2310,13 +2337,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>34960</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>369570</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2916553</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>2038351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2371,13 +2398,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>122468</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2836545</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>2804159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2432,13 +2459,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>48216</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>196215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2949019</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>2192655</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2493,13 +2520,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>929640</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2343150</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>2419620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2554,13 +2581,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>144934</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2884170</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>2836544</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2615,13 +2642,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2872740</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>2819400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2676,13 +2703,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>52593</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2939878</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>2491741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2737,13 +2764,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2941320</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>1615440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2798,13 +2825,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2918460</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>2514600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2859,13 +2886,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>137159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2937472</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>2636520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2920,13 +2947,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>88777</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>36918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2892640</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>8203</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2981,13 +3008,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>579121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2933700</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>2249857</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3042,13 +3069,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2651760</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>3246120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3103,13 +3130,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>43195</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>205740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>571</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>3086100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3221,16 +3248,134 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>40996</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>140563</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1448916</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8420C5D3-754C-0CA6-A550-6D9C6BE51A43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="8770" t="32482" r="8174" b="30450"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9658472" y="24724311"/>
+          <a:ext cx="2925625" cy="1308353"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133165</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>32000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2766231</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1664563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EA46268-E041-F9C7-E808-759C608A0ED3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9750641" y="26324699"/>
+          <a:ext cx="2633066" cy="1632563"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01071C9A-1503-4F8F-82F4-AA89C87CDE83}" name="Table1" displayName="Table1" ref="A4:J34" totalsRowCount="1" headerRowDxfId="10" dataDxfId="19" totalsRowDxfId="18">
-  <autoFilter ref="A4:J33" xr:uid="{01071C9A-1503-4F8F-82F4-AA89C87CDE83}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01071C9A-1503-4F8F-82F4-AA89C87CDE83}" name="Table1" displayName="Table1" ref="A4:J36" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18" totalsRowDxfId="17">
+  <autoFilter ref="A4:J35" xr:uid="{01071C9A-1503-4F8F-82F4-AA89C87CDE83}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3243,18 +3388,18 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{89BB1A7E-1426-47CD-A275-E013BEAFB9CE}" name="STT" totalsRowLabel="Tổng" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{08A4D493-021D-4B23-B615-32640E1F321D}" name="Tên Linh Kiện" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{2AE88D82-FF90-4B55-BF62-93E5BC44042D}" name="Thông số kỹ thuật" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{170CAB26-31F1-40E8-851D-7C813AF43EA3}" name="Giá Tiền" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{33637D27-AAE2-42A8-A7DD-E6E98249494C}" name="Số Lượng" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{5BB60D2A-D62C-4DAC-A643-73A49C02CCD3}" name="Đơn Vị " dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{5E2743AD-1852-4AD7-8E8F-D253BF2337CC}" name="Thành Tiền" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="1" xr3:uid="{89BB1A7E-1426-47CD-A275-E013BEAFB9CE}" name="STT" totalsRowLabel="Tổng" dataDxfId="16" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{08A4D493-021D-4B23-B615-32640E1F321D}" name="Tên Linh Kiện" dataDxfId="15" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{2AE88D82-FF90-4B55-BF62-93E5BC44042D}" name="Thông số kỹ thuật" dataDxfId="14" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{170CAB26-31F1-40E8-851D-7C813AF43EA3}" name="Giá Tiền" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{33637D27-AAE2-42A8-A7DD-E6E98249494C}" name="Số Lượng" dataDxfId="12" totalsRowDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{5BB60D2A-D62C-4DAC-A643-73A49C02CCD3}" name="Đơn Vị " dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{5E2743AD-1852-4AD7-8E8F-D253BF2337CC}" name="Thành Tiền" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D612B1E0-40EA-4BA3-BFA5-FB91B71D1EFC}" name="Hình Ảnh" totalsRowDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{EEC95CE9-D4D6-4B60-9868-8D82ADE756E7}" name="Link Sản Phẩm" totalsRowDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{61E4AC14-42B6-41E9-9B99-7D7B661363A8}" name="Ghi Chú" totalsRowDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{D612B1E0-40EA-4BA3-BFA5-FB91B71D1EFC}" name="Hình Ảnh" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{EEC95CE9-D4D6-4B60-9868-8D82ADE756E7}" name="Link Sản Phẩm" totalsRowDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{61E4AC14-42B6-41E9-9B99-7D7B661363A8}" name="Ghi Chú" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3557,21 +3702,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA65EB4-8289-4119-A8F9-E941FA854F49}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="103" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="42" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" style="31" customWidth="1"/>
+    <col min="1" max="1" width="7" style="30" customWidth="1"/>
     <col min="2" max="2" width="23.77734375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="31" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="30" customWidth="1"/>
     <col min="8" max="8" width="43.21875" style="1" customWidth="1"/>
     <col min="9" max="9" width="34.21875" style="2" customWidth="1"/>
     <col min="10" max="10" width="23.33203125" style="8" customWidth="1"/>
@@ -3579,42 +3724,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
@@ -3658,7 +3803,7 @@
       <c r="C5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>810000</v>
       </c>
       <c r="E5" s="13">
@@ -3667,7 +3812,7 @@
       <c r="F5" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>810000</v>
       </c>
@@ -3689,7 +3834,7 @@
       <c r="C6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>650000</v>
       </c>
       <c r="E6" s="13">
@@ -3698,7 +3843,7 @@
       <c r="F6" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>5200000</v>
       </c>
@@ -3720,7 +3865,7 @@
       <c r="C7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>1085000</v>
       </c>
       <c r="E7" s="13">
@@ -3729,7 +3874,7 @@
       <c r="F7" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>1085000</v>
       </c>
@@ -3751,7 +3896,7 @@
       <c r="C8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>1650000</v>
       </c>
       <c r="E8" s="13">
@@ -3760,7 +3905,7 @@
       <c r="F8" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>6600000</v>
       </c>
@@ -3782,7 +3927,7 @@
       <c r="C9" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>235000</v>
       </c>
       <c r="E9" s="13">
@@ -3791,7 +3936,7 @@
       <c r="F9" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>235000</v>
       </c>
@@ -3813,7 +3958,7 @@
       <c r="C10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>1150000</v>
       </c>
       <c r="E10" s="13">
@@ -3822,7 +3967,7 @@
       <c r="F10" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>2300000</v>
       </c>
@@ -3844,7 +3989,7 @@
       <c r="C11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>16000000</v>
       </c>
       <c r="E11" s="13">
@@ -3853,7 +3998,7 @@
       <c r="F11" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>64000000</v>
       </c>
@@ -3875,7 +4020,7 @@
       <c r="C12" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>370000</v>
       </c>
       <c r="E12" s="13">
@@ -3884,7 +4029,7 @@
       <c r="F12" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>370000</v>
       </c>
@@ -3906,7 +4051,7 @@
       <c r="C13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>155000</v>
       </c>
       <c r="E13" s="13">
@@ -3915,7 +4060,7 @@
       <c r="F13" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>155000</v>
       </c>
@@ -3927,18 +4072,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>10</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="32">
-        <v>17600000</v>
+        <v>138</v>
+      </c>
+      <c r="D14" s="31">
+        <v>4800000</v>
       </c>
       <c r="E14" s="13">
         <v>1</v>
@@ -3946,623 +4091,681 @@
       <c r="F14" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
+        <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
+        <v>4800000</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="31">
+        <v>10000000</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" s="31">
+        <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
+        <v>20000000</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>12</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="31">
+        <v>17600000</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>17600000</v>
       </c>
-      <c r="H14"/>
-      <c r="I14" s="9" t="s">
+      <c r="H16"/>
+      <c r="I16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
-        <v>11</v>
-      </c>
-      <c r="B15" s="15" t="s">
+    <row r="17" spans="1:10" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>13</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C17" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D17" s="31">
         <v>11900000</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E17" s="13">
         <v>1</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G17" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>11900000</v>
       </c>
-      <c r="H15"/>
-      <c r="I15" s="9" t="s">
+      <c r="H17"/>
+      <c r="I17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J17" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="202.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <v>12</v>
-      </c>
-      <c r="B16" s="15" t="s">
+    <row r="18" spans="1:10" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>14</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D18" s="31">
         <v>700000</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E18" s="13">
         <v>4</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G18" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>2800000</v>
       </c>
-      <c r="H16"/>
-      <c r="I16" s="9" t="s">
+      <c r="H18"/>
+      <c r="I18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="212.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
-        <v>13</v>
-      </c>
-      <c r="B17" s="16" t="s">
+    <row r="19" spans="1:10" ht="212.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
+        <v>15</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C19" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D19" s="33">
         <v>750000</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E19" s="17">
         <v>2</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G19" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>1500000</v>
       </c>
-      <c r="H17"/>
-      <c r="I17" s="9" t="s">
+      <c r="H19"/>
+      <c r="I19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="234" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
-        <v>14</v>
-      </c>
-      <c r="B18" s="16" t="s">
+    <row r="20" spans="1:10" ht="234" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>16</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C20" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D20" s="33">
         <v>4650000</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E20" s="17">
         <v>1</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F20" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G20" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>4650000</v>
       </c>
-      <c r="H18"/>
-      <c r="I18" s="9" t="s">
+      <c r="H20"/>
+      <c r="I20" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J20" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
-        <v>15</v>
-      </c>
-      <c r="B19" s="16" t="s">
+    <row r="21" spans="1:10" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
+        <v>17</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C21" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D21" s="33">
         <v>2750000</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E21" s="17">
         <v>1</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G21" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>2750000</v>
       </c>
-      <c r="H19"/>
-      <c r="I19" s="9" t="s">
+      <c r="H21"/>
+      <c r="I21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J21" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
-        <v>16</v>
-      </c>
-      <c r="B20" s="16" t="s">
+    <row r="22" spans="1:10" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <v>18</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C22" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D22" s="33">
         <v>35000</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E22" s="17">
         <v>1</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G22" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>35000</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="9" t="s">
+      <c r="H22" s="6"/>
+      <c r="I22" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J22" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
-        <v>17</v>
-      </c>
-      <c r="B21" s="16" t="s">
+    <row r="23" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
+        <v>19</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C23" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D23" s="33">
         <v>21000</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E23" s="17">
         <v>2</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G23" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>42000</v>
       </c>
-      <c r="H21"/>
-      <c r="I21" s="9" t="s">
+      <c r="H23"/>
+      <c r="I23" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J23" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
-        <v>18</v>
-      </c>
-      <c r="B22" s="16" t="s">
+    <row r="24" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
+        <v>20</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C24" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D24" s="33">
         <v>55000</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E24" s="17">
         <v>3</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G24" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>165000</v>
       </c>
-      <c r="H22"/>
-      <c r="I22" s="9" t="s">
+      <c r="H24"/>
+      <c r="I24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
-        <v>19</v>
-      </c>
-      <c r="B23" s="16" t="s">
+    <row r="25" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
+        <v>21</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C25" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D25" s="33">
         <v>40000</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E25" s="17">
         <v>2</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F25" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G25" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>80000</v>
       </c>
-      <c r="H23"/>
-      <c r="I23" s="9" t="s">
+      <c r="H25"/>
+      <c r="I25" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J25" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="224.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
-        <v>20</v>
-      </c>
-      <c r="B24" s="16" t="s">
+    <row r="26" spans="1:10" ht="224.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13">
+        <v>22</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C26" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D26" s="33">
         <v>55000</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E26" s="17">
         <v>3</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G26" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>165000</v>
       </c>
-      <c r="H24"/>
-      <c r="I24" s="9" t="s">
+      <c r="H26"/>
+      <c r="I26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J26" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="227.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
-        <v>21</v>
-      </c>
-      <c r="B25" s="16" t="s">
+    <row r="27" spans="1:10" ht="227.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
+        <v>23</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C27" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D27" s="33">
         <v>101062</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E27" s="17">
         <v>3</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G27" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>303186</v>
       </c>
-      <c r="H25"/>
-      <c r="I25" s="9" t="s">
+      <c r="H27"/>
+      <c r="I27" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J27" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="202.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
-        <v>22</v>
-      </c>
-      <c r="B26" s="16" t="s">
+    <row r="28" spans="1:10" ht="202.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
+        <v>24</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C28" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D28" s="33">
         <v>7000</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E28" s="17">
         <v>6</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G28" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>42000</v>
       </c>
-      <c r="H26"/>
-      <c r="I26" s="9" t="s">
+      <c r="H28"/>
+      <c r="I28" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J28" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="166.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13">
-        <v>23</v>
-      </c>
-      <c r="B27" s="16" t="s">
+    <row r="29" spans="1:10" ht="166.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <v>25</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C29" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D29" s="33">
         <v>100000</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E29" s="17">
         <v>1</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G29" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>100000</v>
       </c>
-      <c r="H27"/>
-      <c r="I27" s="9" t="s">
+      <c r="H29"/>
+      <c r="I29" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="J29" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="199.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
-        <v>24</v>
-      </c>
-      <c r="B28" s="16" t="s">
+    <row r="30" spans="1:10" ht="199.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>26</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C30" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D30" s="33">
         <v>25000</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E30" s="17">
         <v>3</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G30" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>75000</v>
       </c>
-      <c r="H28"/>
-      <c r="I28" s="9" t="s">
+      <c r="H30"/>
+      <c r="I30" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J30" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
-        <v>25</v>
-      </c>
-      <c r="B29" s="15" t="s">
+    <row r="31" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>27</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C31" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D31" s="31">
         <v>65000</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E31" s="13">
         <v>1</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G31" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>65000</v>
       </c>
-      <c r="H29"/>
-      <c r="I29" s="9" t="s">
+      <c r="H31"/>
+      <c r="I31" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
-        <v>26</v>
-      </c>
-      <c r="B30" s="15" t="s">
+    <row r="32" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <v>28</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C32" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D32" s="31">
         <v>52000</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E32" s="13">
         <v>1</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F32" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G32" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>52000</v>
       </c>
-      <c r="H30"/>
-      <c r="I30" s="9" t="s">
+      <c r="H32"/>
+      <c r="I32" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
-        <v>27</v>
-      </c>
-      <c r="B31" s="15" t="s">
+    <row r="33" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
+        <v>29</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C33" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D33" s="31">
         <v>85000</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E33" s="13">
         <v>1</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="32">
+      <c r="G33" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>85000</v>
       </c>
-      <c r="H31"/>
-      <c r="I31" s="9" t="s">
+      <c r="H33"/>
+      <c r="I33" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="257.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
-        <v>28</v>
-      </c>
-      <c r="B32" s="15" t="s">
+    <row r="34" spans="1:10" ht="257.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>30</v>
+      </c>
+      <c r="B34" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C34" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D34" s="31">
         <v>5650000</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E34" s="13">
         <v>1</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F34" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="32">
+      <c r="G34" s="31">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>5650000</v>
       </c>
-      <c r="H32"/>
-      <c r="I32" s="10" t="s">
+      <c r="H34"/>
+      <c r="I34" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="261.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
-        <v>29</v>
-      </c>
-      <c r="B33" s="16" t="s">
+    <row r="35" spans="1:10" ht="261.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>31</v>
+      </c>
+      <c r="B35" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C35" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D35" s="33">
         <v>80000</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E35" s="34">
         <v>3</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F35" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G35" s="33">
         <f>Table1[[#This Row],[Giá Tiền]]*Table1[[#This Row],[Số Lượng]]</f>
         <v>240000</v>
       </c>
-      <c r="H33"/>
-      <c r="I33" s="9" t="s">
+      <c r="H35"/>
+      <c r="I35" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="J35" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="30" t="s">
+    <row r="36" spans="1:10" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="36">
+      <c r="B36" s="18"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="35">
         <f>SUBTOTAL(109,Table1[Thành Tiền])</f>
-        <v>129054186</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
+        <v>153854186</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4576,22 +4779,23 @@
     <hyperlink ref="C11" r:id="rId4" xr:uid="{68B3911F-281E-42E3-9CDE-4D949DBEFC9D}"/>
     <hyperlink ref="I11" r:id="rId5" xr:uid="{2645E4FF-72EA-4D50-A4B9-C915D12ABD6F}"/>
     <hyperlink ref="I13" r:id="rId6" display="https://shopee.vn/-L%E1%BA%ADp-Tr%C3%ACnh-Nh%C3%BAng-A-Z-G92-Kit-Wifi-Esp32-CH340-30P-Type-C-(%C4%90%C3%A3-H%C3%A0n-Ch%C3%A2n)-i.107147748.57701305582?extraParams=%7B%22display_model_id%22%3A370117015224%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=9f2938e5-2361-4f6d-8243-3c040094b675&amp;xptdk=9f2938e5-2361-4f6d-8243-3c040094b675" xr:uid="{CE9F146F-8A76-435C-BFCC-346C8DE7168D}"/>
-    <hyperlink ref="I22" r:id="rId7" display="https://shopee.vn/-HanYong-Nux-N%C3%BAt-d%E1%BB%ABng-kh%E1%BA%A9n-c%E1%BA%A5p-phi-30-CRE-30R1R-Hanyoung-i.953709471.23586525546?extraParams=%7B%22display_model_id%22%3A157111264318%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=3732b115-c9ff-4c90-a46f-0268ec730f72&amp;xptdk=3732b115-c9ff-4c90-a46f-0268ec730f72" xr:uid="{7F10230E-4329-4F04-A675-4F88B9DC3967}"/>
-    <hyperlink ref="I14" r:id="rId8" xr:uid="{8BCF0FC6-A4ED-48AD-9005-091B45837371}"/>
-    <hyperlink ref="I17" r:id="rId9" xr:uid="{02502F88-4BEE-41E9-9AA5-1CC5030F32C6}"/>
-    <hyperlink ref="I33" r:id="rId10" display="https://shopee.vn/Domino-c%E1%BA%A7u-%C4%91%E1%BA%A5u-%C4%91i%E1%BB%87n-10A-20A-30A-60A-Hanyoung-Nux-(t%E1%BB%91t)-h%C3%A0n-qu%E1%BB%91c-i.275475149.15099489307?extraParams=%7B%22display_model_id%22%3A207036529885%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=38f3afc2-3591-439d-bf18-144afc3ed552&amp;xptdk=38f3afc2-3591-439d-bf18-144afc3ed552" xr:uid="{3C533595-C5FA-4C5C-A30B-A97BDEB6E98A}"/>
-    <hyperlink ref="I30" r:id="rId11" display="https://shopee.vn/C%E1%BA%A7u-Ch%C3%AC-%E1%BB%90ng-5x20mm-(-c%C3%A1c-s%E1%BB%91-)-i.889077761.22753685206?extraParams=%7B%22display_model_id%22%3A184556463915%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=bfa94b1c-27ed-497d-8b6e-3e482f4fc497&amp;xptdk=bfa94b1c-27ed-497d-8b6e-3e482f4fc497" xr:uid="{0D1D3BC4-DBA3-4473-90CF-23F1E59C8BD1}"/>
-    <hyperlink ref="I23" r:id="rId12" xr:uid="{14E212F1-CD83-4AB6-B072-0F4EE289B701}"/>
+    <hyperlink ref="I24" r:id="rId7" display="https://shopee.vn/-HanYong-Nux-N%C3%BAt-d%E1%BB%ABng-kh%E1%BA%A9n-c%E1%BA%A5p-phi-30-CRE-30R1R-Hanyoung-i.953709471.23586525546?extraParams=%7B%22display_model_id%22%3A157111264318%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=3732b115-c9ff-4c90-a46f-0268ec730f72&amp;xptdk=3732b115-c9ff-4c90-a46f-0268ec730f72" xr:uid="{7F10230E-4329-4F04-A675-4F88B9DC3967}"/>
+    <hyperlink ref="I16" r:id="rId8" xr:uid="{8BCF0FC6-A4ED-48AD-9005-091B45837371}"/>
+    <hyperlink ref="I19" r:id="rId9" xr:uid="{02502F88-4BEE-41E9-9AA5-1CC5030F32C6}"/>
+    <hyperlink ref="I35" r:id="rId10" display="https://shopee.vn/Domino-c%E1%BA%A7u-%C4%91%E1%BA%A5u-%C4%91i%E1%BB%87n-10A-20A-30A-60A-Hanyoung-Nux-(t%E1%BB%91t)-h%C3%A0n-qu%E1%BB%91c-i.275475149.15099489307?extraParams=%7B%22display_model_id%22%3A207036529885%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=38f3afc2-3591-439d-bf18-144afc3ed552&amp;xptdk=38f3afc2-3591-439d-bf18-144afc3ed552" xr:uid="{3C533595-C5FA-4C5C-A30B-A97BDEB6E98A}"/>
+    <hyperlink ref="I32" r:id="rId11" display="https://shopee.vn/C%E1%BA%A7u-Ch%C3%AC-%E1%BB%90ng-5x20mm-(-c%C3%A1c-s%E1%BB%91-)-i.889077761.22753685206?extraParams=%7B%22display_model_id%22%3A184556463915%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=bfa94b1c-27ed-497d-8b6e-3e482f4fc497&amp;xptdk=bfa94b1c-27ed-497d-8b6e-3e482f4fc497" xr:uid="{0D1D3BC4-DBA3-4473-90CF-23F1E59C8BD1}"/>
+    <hyperlink ref="I25" r:id="rId12" xr:uid="{14E212F1-CD83-4AB6-B072-0F4EE289B701}"/>
     <hyperlink ref="I9" r:id="rId13" display="https://shopee.vn/%C4%90%E1%BA%BF-ra-ch%C3%A2n-stm32f4-lo%E1%BA%A1i-domino-2-t%E1%BA%A7ng-3.81mm-i.1404458001.29383391281?extraParams=%7B%22display_model_id%22%3A147794153017%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=8163c000-2f34-437a-bb3a-971355a4cf99&amp;xptdk=8163c000-2f34-437a-bb3a-971355a4cf99" xr:uid="{531C5858-3EB4-4F8E-8542-D5DD6810E63F}"/>
-    <hyperlink ref="I15" r:id="rId14" xr:uid="{B7DBF328-B38A-4A02-9809-BC2F41C99EDF}"/>
-    <hyperlink ref="I16" r:id="rId15" xr:uid="{F24AC75B-2503-4658-AE8F-BDE855CD6AB4}"/>
-    <hyperlink ref="I18" r:id="rId16" xr:uid="{6D9342AA-36B8-41AE-8F28-4562E5337F6A}"/>
+    <hyperlink ref="I17" r:id="rId14" xr:uid="{B7DBF328-B38A-4A02-9809-BC2F41C99EDF}"/>
+    <hyperlink ref="I18" r:id="rId15" xr:uid="{F24AC75B-2503-4658-AE8F-BDE855CD6AB4}"/>
+    <hyperlink ref="I20" r:id="rId16" xr:uid="{6D9342AA-36B8-41AE-8F28-4562E5337F6A}"/>
+    <hyperlink ref="I14" r:id="rId17" xr:uid="{EEF13C03-604A-4C22-BAF9-958735991A69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
-  <drawing r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
+  <drawing r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>